<commit_message>
updated peak detector error plots
</commit_message>
<xml_diff>
--- a/self-tuning-buck-converter/Peak Detector/Evaluation/Peak Detector Evaluation.xlsx
+++ b/self-tuning-buck-converter/Peak Detector/Evaluation/Peak Detector Evaluation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\state-opera.ecs.vuw.ac.nz\claytoniel\Desktop\Uni-Notes\self-tuning-buck-converter\self-tuning-buck-converter\Peak Detector\Evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2275D99C-3A79-4373-AB90-50655D2E5DC5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408A6D30-7BBD-4E0A-B6F3-CF3DAE575E87}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{C1352C5F-0847-4A0F-B095-DF52534FE8DE}"/>
   </bookViews>
@@ -159,22 +159,22 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1718,38 +1718,18 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-NZ" sz="1400" b="0" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
+              <a:rPr lang="en-NZ"/>
               <a:t>Peak to Peak Voltage Measurment Error %</a:t>
             </a:r>
-            <a:endParaRPr lang="en-NZ" sz="1400">
-              <a:effectLst/>
-            </a:endParaRPr>
           </a:p>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
+              <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-NZ" sz="1400" b="0" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
+              <a:rPr lang="en-NZ"/>
               <a:t> Peak Voltage = 1500mV</a:t>
             </a:r>
-            <a:endParaRPr lang="en-NZ" sz="1400">
-              <a:effectLst/>
-            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1761,6 +1741,26 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1774,6 +1774,15 @@
           <c:tx>
             <c:v>First Design</c:v>
           </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
             <c:size val="5"/>
@@ -1946,6 +1955,30 @@
           <c:tx>
             <c:v>Improved Design</c:v>
           </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$I$7:$I$27</c:f>
@@ -2150,14 +2183,9 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-NZ" sz="1000"/>
-                  <a:t>PWM</a:t>
+                  <a:rPr lang="en-NZ"/>
+                  <a:t>PWM Frequency (kHz)</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-NZ" sz="1000" baseline="0"/>
-                  <a:t> Frequency (kHz)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-NZ" sz="800"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -2169,6 +2197,26 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -2253,13 +2301,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-NZ"/>
-                  <a:t>Measurment</a:t>
+                  <a:t>Measurment Error (%)</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-NZ" baseline="0"/>
-                  <a:t> Error (%)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-NZ"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -2271,6 +2314,26 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -2313,6 +2376,13 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
@@ -2350,6 +2420,21 @@
     <c:showDLblsOverMax val="0"/>
     <c:extLst/>
   </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
   <c:txPr>
     <a:bodyPr/>
     <a:lstStyle/>
@@ -2967,6 +3052,7 @@
         <c:axId val="968697056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -3794,6 +3880,7 @@
         <c:axId val="971795712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -3856,6 +3943,7 @@
         <c:axId val="1065078688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -4117,6 +4205,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -5150,6 +5278,522 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6151,8 +6795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{546694CF-224D-485F-9D28-7577BCAB77AB}">
   <dimension ref="A1:W27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W7" activeCellId="6" sqref="A7:A27 D7:D27 L7:L27 T7:T27 G7:G26 O7:O27 W7:W27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6180,161 +6824,161 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="I1" s="1" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="I1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="Q1" s="1" t="s">
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="Q1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
+      <c r="B2" s="9"/>
       <c r="C2">
         <v>150</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="3"/>
+      <c r="J2" s="9"/>
       <c r="K2">
         <v>500</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="R2" s="3"/>
+      <c r="R2" s="9"/>
       <c r="S2">
         <v>1500</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="10"/>
       <c r="C3">
         <f>(C2/2)</f>
         <v>75</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="4"/>
+      <c r="J3" s="10"/>
       <c r="K3">
         <f>(K2/2)</f>
         <v>250</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="Q3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="R3" s="4"/>
+      <c r="R3" s="10"/>
       <c r="S3">
         <f>(S2/2)</f>
         <v>750</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="5">
+      <c r="B4" s="10"/>
+      <c r="C4" s="2">
         <v>5999.9</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="4"/>
-      <c r="K4" s="5">
+      <c r="J4" s="10"/>
+      <c r="K4" s="2">
         <v>6002.2</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="Q4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="R4" s="4"/>
-      <c r="S4" s="5">
+      <c r="R4" s="10"/>
+      <c r="S4" s="2">
         <v>6001.7</v>
       </c>
     </row>
     <row r="5" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="6" t="s">
+      <c r="H6" s="1"/>
+      <c r="I6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="K6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="L6" s="10" t="s">
+      <c r="L6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="M6" s="7" t="s">
+      <c r="M6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="N6" s="7" t="s">
+      <c r="N6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="O6" s="8" t="s">
+      <c r="O6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="Q6" s="6" t="s">
+      <c r="Q6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="R6" s="7" t="s">
+      <c r="R6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="S6" s="7" t="s">
+      <c r="S6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="T6" s="10" t="s">
+      <c r="T6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="U6" s="7" t="s">
+      <c r="U6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="V6" s="7" t="s">
+      <c r="V6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="W6" s="8" t="s">
+      <c r="W6" s="5" t="s">
         <v>7</v>
       </c>
     </row>
@@ -6342,75 +6986,75 @@
       <c r="A7">
         <v>1</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="2">
         <v>6078.8</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="2">
         <f>((C4+C3) - B7)</f>
         <v>-3.9000000000005457</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="6">
         <f>(C7/75)*100</f>
         <v>-5.2000000000007276</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="2">
         <v>6071.5</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="2">
         <f>((C4+C3) - E7)</f>
         <v>3.3999999999996362</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="6">
         <f>(F7/75)*100</f>
         <v>4.5333333333328483</v>
       </c>
       <c r="I7">
         <v>1</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7" s="2">
         <v>6253.8</v>
       </c>
-      <c r="K7" s="5">
+      <c r="K7" s="2">
         <f>((K4+K3) - J7)</f>
         <v>-1.6000000000003638</v>
       </c>
-      <c r="L7" s="9">
+      <c r="L7" s="6">
         <f>(K7/250)*100</f>
         <v>-0.64000000000014545</v>
       </c>
-      <c r="M7" s="5">
+      <c r="M7" s="2">
         <v>6245.2</v>
       </c>
-      <c r="N7" s="5">
+      <c r="N7" s="2">
         <f>((K4+K3) - M7)</f>
         <v>7</v>
       </c>
-      <c r="O7" s="9">
+      <c r="O7" s="6">
         <f>(N7/250)*100</f>
         <v>2.8000000000000003</v>
       </c>
       <c r="Q7">
         <v>1</v>
       </c>
-      <c r="R7" s="5">
+      <c r="R7" s="2">
         <v>6746.3</v>
       </c>
-      <c r="S7" s="5">
+      <c r="S7" s="2">
         <f>((S4+S3) - R7)</f>
         <v>5.3999999999996362</v>
       </c>
-      <c r="T7" s="9">
+      <c r="T7" s="6">
         <f>(S7/750)*100</f>
         <v>0.71999999999995146</v>
       </c>
-      <c r="U7" s="5">
+      <c r="U7" s="2">
         <v>6736.7</v>
       </c>
-      <c r="V7" s="5">
+      <c r="V7" s="2">
         <f>((S4+S3) - U7)</f>
         <v>15</v>
       </c>
-      <c r="W7" s="9">
+      <c r="W7" s="6">
         <f>(V7/750)*100</f>
         <v>2</v>
       </c>
@@ -6419,75 +7063,75 @@
       <c r="A8">
         <v>5</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="2">
         <v>6078.7</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="2">
         <f>((C4+C3) - B8)</f>
         <v>-3.8000000000001819</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="6">
         <f t="shared" ref="D8:D27" si="0">(C8/75)*100</f>
         <v>-5.0666666666669098</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="2">
         <v>6069.1</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="2">
         <f>((C4+C3) - E8)</f>
         <v>5.7999999999992724</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="6">
         <f t="shared" ref="G8:G27" si="1">(F8/75)*100</f>
         <v>7.7333333333323635</v>
       </c>
       <c r="I8">
         <v>5</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J8" s="2">
         <v>6253.9</v>
       </c>
-      <c r="K8" s="5">
+      <c r="K8" s="2">
         <f>((K4+K3) - J8)</f>
         <v>-1.6999999999998181</v>
       </c>
-      <c r="L8" s="9">
+      <c r="L8" s="6">
         <f t="shared" ref="L8:L27" si="2">(K8/250)*100</f>
         <v>-0.67999999999992733</v>
       </c>
-      <c r="M8" s="5">
+      <c r="M8" s="2">
         <v>6237.2</v>
       </c>
-      <c r="N8" s="5">
+      <c r="N8" s="2">
         <f>((K4+K3) - M8)</f>
         <v>15</v>
       </c>
-      <c r="O8" s="9">
+      <c r="O8" s="6">
         <f t="shared" ref="O8:O27" si="3">(N8/250)*100</f>
         <v>6</v>
       </c>
       <c r="Q8">
         <v>5</v>
       </c>
-      <c r="R8" s="5">
+      <c r="R8" s="2">
         <v>6746</v>
       </c>
-      <c r="S8" s="5">
+      <c r="S8" s="2">
         <f>((S4+S3) - R8)</f>
         <v>5.6999999999998181</v>
       </c>
-      <c r="T8" s="9">
+      <c r="T8" s="6">
         <f t="shared" ref="T8:T27" si="4">(S8/750)*100</f>
         <v>0.75999999999997569</v>
       </c>
-      <c r="U8" s="5">
+      <c r="U8" s="2">
         <v>6722</v>
       </c>
-      <c r="V8" s="5">
+      <c r="V8" s="2">
         <f>((S4+S3) - U8)</f>
         <v>29.699999999999818</v>
       </c>
-      <c r="W8" s="9">
+      <c r="W8" s="6">
         <f t="shared" ref="W8:W27" si="5">(V8/750)*100</f>
         <v>3.959999999999976</v>
       </c>
@@ -6496,75 +7140,75 @@
       <c r="A9">
         <v>10</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="2">
         <v>6078.6</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="2">
         <f>((C4+C3) - B9)</f>
         <v>-3.7000000000007276</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="6">
         <f t="shared" si="0"/>
         <v>-4.9333333333343035</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="2">
         <v>6062.1</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="2">
         <f>((C4+C3) - E9)</f>
         <v>12.799999999999272</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="6">
         <f t="shared" si="1"/>
         <v>17.066666666665697</v>
       </c>
       <c r="I9">
         <v>10</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J9" s="2">
         <v>6254.1</v>
       </c>
-      <c r="K9" s="5">
+      <c r="K9" s="2">
         <f>((K4+K3) - J9)</f>
         <v>-1.9000000000005457</v>
       </c>
-      <c r="L9" s="9">
+      <c r="L9" s="6">
         <f t="shared" si="2"/>
         <v>-0.76000000000021828</v>
       </c>
-      <c r="M9" s="5">
+      <c r="M9" s="2">
         <v>6228.3</v>
       </c>
-      <c r="N9" s="5">
+      <c r="N9" s="2">
         <f>((K4+K3) - M9)</f>
         <v>23.899999999999636</v>
       </c>
-      <c r="O9" s="9">
+      <c r="O9" s="6">
         <f t="shared" si="3"/>
         <v>9.5599999999998548</v>
       </c>
       <c r="Q9">
         <v>10</v>
       </c>
-      <c r="R9" s="5">
+      <c r="R9" s="2">
         <v>6748.1</v>
       </c>
-      <c r="S9" s="5">
+      <c r="S9" s="2">
         <f>((S4+S3) - R9)</f>
         <v>3.5999999999994543</v>
       </c>
-      <c r="T9" s="9">
+      <c r="T9" s="6">
         <f t="shared" si="4"/>
         <v>0.47999999999992726</v>
       </c>
-      <c r="U9" s="5">
+      <c r="U9" s="2">
         <v>6710</v>
       </c>
-      <c r="V9" s="5">
+      <c r="V9" s="2">
         <f>((S4+S3) - U9)</f>
         <v>41.699999999999818</v>
       </c>
-      <c r="W9" s="9">
+      <c r="W9" s="6">
         <f t="shared" si="5"/>
         <v>5.5599999999999756</v>
       </c>
@@ -6573,75 +7217,75 @@
       <c r="A10">
         <v>15</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="2">
         <v>6077.8</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="2">
         <f>((C4+C3) - B10)</f>
         <v>-2.9000000000005457</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="6">
         <f t="shared" si="0"/>
         <v>-3.8666666666673941</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="2">
         <v>6056.4</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="2">
         <f>((C4+C3) - E10)</f>
         <v>18.5</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="6">
         <f t="shared" si="1"/>
         <v>24.666666666666668</v>
       </c>
       <c r="I10">
         <v>15</v>
       </c>
-      <c r="J10" s="5">
+      <c r="J10" s="2">
         <v>6252.7</v>
       </c>
-      <c r="K10" s="5">
+      <c r="K10" s="2">
         <f>((K4+K3) - J10)</f>
         <v>-0.5</v>
       </c>
-      <c r="L10" s="9">
+      <c r="L10" s="6">
         <f t="shared" si="2"/>
         <v>-0.2</v>
       </c>
-      <c r="M10" s="5">
+      <c r="M10" s="2">
         <v>6219.3</v>
       </c>
-      <c r="N10" s="5">
+      <c r="N10" s="2">
         <f>((K4+K3) - M10)</f>
         <v>32.899999999999636</v>
       </c>
-      <c r="O10" s="9">
+      <c r="O10" s="6">
         <f t="shared" si="3"/>
         <v>13.159999999999854</v>
       </c>
       <c r="Q10">
         <v>15</v>
       </c>
-      <c r="R10" s="5">
+      <c r="R10" s="2">
         <v>6745.2</v>
       </c>
-      <c r="S10" s="5">
+      <c r="S10" s="2">
         <f>((S4+S3) - R10)</f>
         <v>6.5</v>
       </c>
-      <c r="T10" s="9">
+      <c r="T10" s="6">
         <f t="shared" si="4"/>
         <v>0.86666666666666659</v>
       </c>
-      <c r="U10" s="5">
+      <c r="U10" s="2">
         <v>6695.8</v>
       </c>
-      <c r="V10" s="5">
+      <c r="V10" s="2">
         <f>((S4+S3) - U10)</f>
         <v>55.899999999999636</v>
       </c>
-      <c r="W10" s="9">
+      <c r="W10" s="6">
         <f t="shared" si="5"/>
         <v>7.4533333333332852</v>
       </c>
@@ -6650,75 +7294,75 @@
       <c r="A11">
         <v>20</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="2">
         <v>6077.1</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="2">
         <f>((C4+C3) - B11)</f>
         <v>-2.2000000000007276</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="6">
         <f t="shared" si="0"/>
         <v>-2.9333333333343035</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="2">
         <v>6051.6</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="2">
         <f>((C4+C3) - E11)</f>
         <v>23.299999999999272</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="6">
         <f t="shared" si="1"/>
         <v>31.0666666666657</v>
       </c>
       <c r="I11">
         <v>20</v>
       </c>
-      <c r="J11" s="5">
+      <c r="J11" s="2">
         <v>6250.8</v>
       </c>
-      <c r="K11" s="5">
+      <c r="K11" s="2">
         <f>((K4+K3) - J11)</f>
         <v>1.3999999999996362</v>
       </c>
-      <c r="L11" s="9">
+      <c r="L11" s="6">
         <f t="shared" si="2"/>
         <v>0.5599999999998545</v>
       </c>
-      <c r="M11" s="5">
+      <c r="M11" s="2">
         <v>6211.5</v>
       </c>
-      <c r="N11" s="5">
+      <c r="N11" s="2">
         <f>((K4+K3) - M11)</f>
         <v>40.699999999999818</v>
       </c>
-      <c r="O11" s="9">
+      <c r="O11" s="6">
         <f t="shared" si="3"/>
         <v>16.279999999999927</v>
       </c>
       <c r="Q11">
         <v>20</v>
       </c>
-      <c r="R11" s="5">
+      <c r="R11" s="2">
         <v>6742.3</v>
       </c>
-      <c r="S11" s="5">
+      <c r="S11" s="2">
         <f>((S4+S3) - R11)</f>
         <v>9.3999999999996362</v>
       </c>
-      <c r="T11" s="9">
+      <c r="T11" s="6">
         <f t="shared" si="4"/>
         <v>1.2533333333332848</v>
       </c>
-      <c r="U11" s="5">
+      <c r="U11" s="2">
         <v>6683</v>
       </c>
-      <c r="V11" s="5">
+      <c r="V11" s="2">
         <f>((S4+S3) - U11)</f>
         <v>68.699999999999818</v>
       </c>
-      <c r="W11" s="9">
+      <c r="W11" s="6">
         <f t="shared" si="5"/>
         <v>9.1599999999999753</v>
       </c>
@@ -6727,75 +7371,75 @@
       <c r="A12">
         <v>25</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="2">
         <v>6076.5</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="2">
         <f>((C4+C3) - B12)</f>
         <v>-1.6000000000003638</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="6">
         <f t="shared" si="0"/>
         <v>-2.1333333333338182</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="2">
         <v>6046.6</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="2">
         <f>((C4+C3) - E12)</f>
         <v>28.299999999999272</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="6">
         <f t="shared" si="1"/>
         <v>37.733333333332361</v>
       </c>
       <c r="I12">
         <v>25</v>
       </c>
-      <c r="J12" s="5">
+      <c r="J12" s="2">
         <v>6249.5</v>
       </c>
-      <c r="K12" s="5">
+      <c r="K12" s="2">
         <f>((K4+K3) - J12)</f>
         <v>2.6999999999998181</v>
       </c>
-      <c r="L12" s="9">
+      <c r="L12" s="6">
         <f t="shared" si="2"/>
         <v>1.0799999999999272</v>
       </c>
-      <c r="M12" s="5">
+      <c r="M12" s="2">
         <v>6204.3</v>
       </c>
-      <c r="N12" s="5">
+      <c r="N12" s="2">
         <f>((K4+K3) - M12)</f>
         <v>47.899999999999636</v>
       </c>
-      <c r="O12" s="9">
+      <c r="O12" s="6">
         <f t="shared" si="3"/>
         <v>19.159999999999854</v>
       </c>
       <c r="Q12">
         <v>25</v>
       </c>
-      <c r="R12" s="5">
+      <c r="R12" s="2">
         <v>6740.1</v>
       </c>
-      <c r="S12" s="5">
+      <c r="S12" s="2">
         <f>((S4+S3) - R12)</f>
         <v>11.599999999999454</v>
       </c>
-      <c r="T12" s="9">
+      <c r="T12" s="6">
         <f t="shared" si="4"/>
         <v>1.546666666666594</v>
       </c>
-      <c r="U12" s="5">
+      <c r="U12" s="2">
         <v>6671.8</v>
       </c>
-      <c r="V12" s="5">
+      <c r="V12" s="2">
         <f>((S4+S3) - U12)</f>
         <v>79.899999999999636</v>
       </c>
-      <c r="W12" s="9">
+      <c r="W12" s="6">
         <f t="shared" si="5"/>
         <v>10.653333333333284</v>
       </c>
@@ -6804,75 +7448,75 @@
       <c r="A13">
         <v>30</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="2">
         <v>6075.8</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="2">
         <f>((C4+C3) - B13)</f>
         <v>-0.9000000000005457</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="6">
         <f t="shared" si="0"/>
         <v>-1.2000000000007276</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="2">
         <v>6042.3</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="2">
         <f>((C4+C3) - E13)</f>
         <v>32.599999999999454</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="6">
         <f t="shared" si="1"/>
         <v>43.466666666665937</v>
       </c>
       <c r="I13">
         <v>30</v>
       </c>
-      <c r="J13" s="5">
+      <c r="J13" s="2">
         <v>6248.9</v>
       </c>
-      <c r="K13" s="5">
+      <c r="K13" s="2">
         <f>((K4+K3) - J13)</f>
         <v>3.3000000000001819</v>
       </c>
-      <c r="L13" s="9">
+      <c r="L13" s="6">
         <f t="shared" si="2"/>
         <v>1.3200000000000727</v>
       </c>
-      <c r="M13" s="5">
+      <c r="M13" s="2">
         <v>6197.8</v>
       </c>
-      <c r="N13" s="5">
+      <c r="N13" s="2">
         <f>((K4+K3) - M13)</f>
         <v>54.399999999999636</v>
       </c>
-      <c r="O13" s="9">
+      <c r="O13" s="6">
         <f t="shared" si="3"/>
         <v>21.759999999999856</v>
       </c>
       <c r="Q13">
         <v>30</v>
       </c>
-      <c r="R13" s="5">
+      <c r="R13" s="2">
         <v>6738.2</v>
       </c>
-      <c r="S13" s="5">
+      <c r="S13" s="2">
         <f>((S4+S3) - R13)</f>
         <v>13.5</v>
       </c>
-      <c r="T13" s="9">
+      <c r="T13" s="6">
         <f t="shared" si="4"/>
         <v>1.7999999999999998</v>
       </c>
-      <c r="U13" s="5">
+      <c r="U13" s="2">
         <v>6661.7</v>
       </c>
-      <c r="V13" s="5">
+      <c r="V13" s="2">
         <f>((S4+S3) - U13)</f>
         <v>90</v>
       </c>
-      <c r="W13" s="9">
+      <c r="W13" s="6">
         <f t="shared" si="5"/>
         <v>12</v>
       </c>
@@ -6881,75 +7525,75 @@
       <c r="A14">
         <v>35</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="2">
         <v>6075.2</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="2">
         <f>((C4+C3) - B14)</f>
         <v>-0.3000000000001819</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="6">
         <f t="shared" si="0"/>
         <v>-0.40000000000024249</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="2">
         <v>6038.4</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="2">
         <f>((C4+C3) - E14)</f>
         <v>36.5</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="6">
         <f t="shared" si="1"/>
         <v>48.666666666666671</v>
       </c>
       <c r="I14">
         <v>35</v>
       </c>
-      <c r="J14" s="5">
+      <c r="J14" s="2">
         <v>6247.8</v>
       </c>
-      <c r="K14" s="5">
+      <c r="K14" s="2">
         <f>((K4+K3) - J14)</f>
         <v>4.3999999999996362</v>
       </c>
-      <c r="L14" s="9">
+      <c r="L14" s="6">
         <f t="shared" si="2"/>
         <v>1.7599999999998543</v>
       </c>
-      <c r="M14" s="5">
+      <c r="M14" s="2">
         <v>6191.6</v>
       </c>
-      <c r="N14" s="5">
+      <c r="N14" s="2">
         <f>((K4+K3) - M14)</f>
         <v>60.599999999999454</v>
       </c>
-      <c r="O14" s="9">
+      <c r="O14" s="6">
         <f t="shared" si="3"/>
         <v>24.239999999999782</v>
       </c>
       <c r="Q14">
         <v>35</v>
       </c>
-      <c r="R14" s="5">
+      <c r="R14" s="2">
         <v>6736.6</v>
       </c>
-      <c r="S14" s="5">
+      <c r="S14" s="2">
         <f>((S4+S3) - R14)</f>
         <v>15.099999999999454</v>
       </c>
-      <c r="T14" s="9">
+      <c r="T14" s="6">
         <f t="shared" si="4"/>
         <v>2.0133333333332604</v>
       </c>
-      <c r="U14" s="5">
+      <c r="U14" s="2">
         <v>6651.8</v>
       </c>
-      <c r="V14" s="5">
+      <c r="V14" s="2">
         <f>((S4+S3) - U14)</f>
         <v>99.899999999999636</v>
       </c>
-      <c r="W14" s="9">
+      <c r="W14" s="6">
         <f t="shared" si="5"/>
         <v>13.319999999999951</v>
       </c>
@@ -6958,75 +7602,75 @@
       <c r="A15">
         <v>40</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="2">
         <v>6074.7</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="2">
         <f>((C4+C3) - B15)</f>
         <v>0.1999999999998181</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="6">
         <f t="shared" si="0"/>
         <v>0.26666666666642413</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="2">
         <v>6034.7</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="2">
         <f>((C4+C3) - E15)</f>
         <v>40.199999999999818</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G15" s="6">
         <f t="shared" si="1"/>
         <v>53.59999999999976</v>
       </c>
       <c r="I15">
         <v>40</v>
       </c>
-      <c r="J15" s="5">
+      <c r="J15" s="2">
         <v>6246.7</v>
       </c>
-      <c r="K15" s="5">
+      <c r="K15" s="2">
         <f>((K4+K3) - J15)</f>
         <v>5.5</v>
       </c>
-      <c r="L15" s="9">
+      <c r="L15" s="6">
         <f t="shared" si="2"/>
         <v>2.1999999999999997</v>
       </c>
-      <c r="M15" s="5">
+      <c r="M15" s="2">
         <v>6185.9</v>
       </c>
-      <c r="N15" s="5">
+      <c r="N15" s="2">
         <f>((K4+K3) - M15)</f>
         <v>66.300000000000182</v>
       </c>
-      <c r="O15" s="9">
+      <c r="O15" s="6">
         <f t="shared" si="3"/>
         <v>26.520000000000071</v>
       </c>
       <c r="Q15">
         <v>40</v>
       </c>
-      <c r="R15" s="5">
+      <c r="R15" s="2">
         <v>6734.5</v>
       </c>
-      <c r="S15" s="5">
+      <c r="S15" s="2">
         <f>((S4+S3) - R15)</f>
         <v>17.199999999999818</v>
       </c>
-      <c r="T15" s="9">
+      <c r="T15" s="6">
         <f t="shared" si="4"/>
         <v>2.293333333333309</v>
       </c>
-      <c r="U15" s="5">
+      <c r="U15" s="2">
         <v>6643</v>
       </c>
-      <c r="V15" s="5">
+      <c r="V15" s="2">
         <f>((S4+S3) - U15)</f>
         <v>108.69999999999982</v>
       </c>
-      <c r="W15" s="9">
+      <c r="W15" s="6">
         <f t="shared" si="5"/>
         <v>14.493333333333307</v>
       </c>
@@ -7035,75 +7679,75 @@
       <c r="A16">
         <v>45</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="2">
         <v>6074.1</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="2">
         <f>((C4+C3) - B16)</f>
         <v>0.7999999999992724</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="6">
         <f t="shared" si="0"/>
         <v>1.0666666666656965</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="2">
         <v>6031.2</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="2">
         <f>((C4+C3) - E16)</f>
         <v>43.699999999999818</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G16" s="6">
         <f t="shared" si="1"/>
         <v>58.266666666666424</v>
       </c>
       <c r="I16">
         <v>45</v>
       </c>
-      <c r="J16" s="5">
+      <c r="J16" s="2">
         <v>6245.9</v>
       </c>
-      <c r="K16" s="5">
+      <c r="K16" s="2">
         <f>((K4+K3) - J16)</f>
         <v>6.3000000000001819</v>
       </c>
-      <c r="L16" s="9">
+      <c r="L16" s="6">
         <f t="shared" si="2"/>
         <v>2.5200000000000728</v>
       </c>
-      <c r="M16" s="5">
+      <c r="M16" s="2">
         <v>6180.3</v>
       </c>
-      <c r="N16" s="5">
+      <c r="N16" s="2">
         <f>((K4+K3) - M16)</f>
         <v>71.899999999999636</v>
       </c>
-      <c r="O16" s="9">
+      <c r="O16" s="6">
         <f t="shared" si="3"/>
         <v>28.759999999999852</v>
       </c>
       <c r="Q16">
         <v>45</v>
       </c>
-      <c r="R16" s="5">
+      <c r="R16" s="2">
         <v>6732.5</v>
       </c>
-      <c r="S16" s="5">
+      <c r="S16" s="2">
         <f>((S4+S3) - R16)</f>
         <v>19.199999999999818</v>
       </c>
-      <c r="T16" s="9">
+      <c r="T16" s="6">
         <f t="shared" si="4"/>
         <v>2.5599999999999756</v>
       </c>
-      <c r="U16" s="5">
+      <c r="U16" s="2">
         <v>6634.5</v>
       </c>
-      <c r="V16" s="5">
+      <c r="V16" s="2">
         <f>((S4+S3) - U16)</f>
         <v>117.19999999999982</v>
       </c>
-      <c r="W16" s="9">
+      <c r="W16" s="6">
         <f t="shared" si="5"/>
         <v>15.626666666666642</v>
       </c>
@@ -7112,75 +7756,75 @@
       <c r="A17">
         <v>50</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="2">
         <v>6073.6</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="2">
         <f>((C4+C3) - B17)</f>
         <v>1.2999999999992724</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="6">
         <f t="shared" si="0"/>
         <v>1.7333333333323633</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="2">
         <v>6027.9</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="2">
         <f>((C4+C3) - E17)</f>
         <v>47</v>
       </c>
-      <c r="G17" s="9">
+      <c r="G17" s="6">
         <f t="shared" si="1"/>
         <v>62.666666666666671</v>
       </c>
       <c r="I17">
         <v>50</v>
       </c>
-      <c r="J17" s="5">
+      <c r="J17" s="2">
         <v>6244.8</v>
       </c>
-      <c r="K17" s="5">
+      <c r="K17" s="2">
         <f>((K4+K3) - J17)</f>
         <v>7.3999999999996362</v>
       </c>
-      <c r="L17" s="9">
+      <c r="L17" s="6">
         <f t="shared" si="2"/>
         <v>2.9599999999998543</v>
       </c>
-      <c r="M17" s="5">
+      <c r="M17" s="2">
         <v>6174.9</v>
       </c>
-      <c r="N17" s="5">
+      <c r="N17" s="2">
         <f>((K4+K3) - M17)</f>
         <v>77.300000000000182</v>
       </c>
-      <c r="O17" s="9">
+      <c r="O17" s="6">
         <f t="shared" si="3"/>
         <v>30.920000000000076</v>
       </c>
       <c r="Q17">
         <v>50</v>
       </c>
-      <c r="R17" s="5">
+      <c r="R17" s="2">
         <v>6731.2</v>
       </c>
-      <c r="S17" s="5">
+      <c r="S17" s="2">
         <f>((S4+S3) - R17)</f>
         <v>20.5</v>
       </c>
-      <c r="T17" s="9">
+      <c r="T17" s="6">
         <f t="shared" si="4"/>
         <v>2.7333333333333334</v>
       </c>
-      <c r="U17" s="5">
+      <c r="U17" s="2">
         <v>6626.2</v>
       </c>
-      <c r="V17" s="5">
+      <c r="V17" s="2">
         <f>((S4+S3) - U17)</f>
         <v>125.5</v>
       </c>
-      <c r="W17" s="9">
+      <c r="W17" s="6">
         <f t="shared" si="5"/>
         <v>16.733333333333334</v>
       </c>
@@ -7189,75 +7833,75 @@
       <c r="A18">
         <v>55</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="2">
         <v>6072.9</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="2">
         <f>((C4+C3) - B18)</f>
         <v>2</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18" s="6">
         <f t="shared" si="0"/>
         <v>2.666666666666667</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="2">
         <v>6024.8</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="2">
         <f>((C4+C3) - E18)</f>
         <v>50.099999999999454</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G18" s="6">
         <f t="shared" si="1"/>
         <v>66.799999999999272</v>
       </c>
       <c r="I18">
         <v>55</v>
       </c>
-      <c r="J18" s="5">
+      <c r="J18" s="2">
         <v>6243.9</v>
       </c>
-      <c r="K18" s="5">
+      <c r="K18" s="2">
         <f>((K4+K3) - J18)</f>
         <v>8.3000000000001819</v>
       </c>
-      <c r="L18" s="9">
+      <c r="L18" s="6">
         <f t="shared" si="2"/>
         <v>3.3200000000000731</v>
       </c>
-      <c r="M18" s="5">
+      <c r="M18" s="2">
         <v>6169.8</v>
       </c>
-      <c r="N18" s="5">
+      <c r="N18" s="2">
         <f>((K4+K3) - M18)</f>
         <v>82.399999999999636</v>
       </c>
-      <c r="O18" s="9">
+      <c r="O18" s="6">
         <f t="shared" si="3"/>
         <v>32.959999999999859</v>
       </c>
       <c r="Q18">
         <v>55</v>
       </c>
-      <c r="R18" s="5">
+      <c r="R18" s="2">
         <v>6729.8</v>
       </c>
-      <c r="S18" s="5">
+      <c r="S18" s="2">
         <f>((S4+S3) - R18)</f>
         <v>21.899999999999636</v>
       </c>
-      <c r="T18" s="9">
+      <c r="T18" s="6">
         <f t="shared" si="4"/>
         <v>2.9199999999999515</v>
       </c>
-      <c r="U18" s="5">
+      <c r="U18" s="2">
         <v>6618.1</v>
       </c>
-      <c r="V18" s="5">
+      <c r="V18" s="2">
         <f>((S4+S3) - U18)</f>
         <v>133.59999999999945</v>
       </c>
-      <c r="W18" s="9">
+      <c r="W18" s="6">
         <f t="shared" si="5"/>
         <v>17.813333333333262</v>
       </c>
@@ -7266,75 +7910,75 @@
       <c r="A19">
         <v>60</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="2">
         <v>6072.3</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="2">
         <f>((C4+C3) - B19)</f>
         <v>2.5999999999994543</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="6">
         <f t="shared" si="0"/>
         <v>3.4666666666659394</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="2">
         <v>6021.9</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F19" s="2">
         <f>((C4+C3) - E19)</f>
         <v>53</v>
       </c>
-      <c r="G19" s="9">
+      <c r="G19" s="6">
         <f t="shared" si="1"/>
         <v>70.666666666666671</v>
       </c>
       <c r="I19">
         <v>60</v>
       </c>
-      <c r="J19" s="5">
+      <c r="J19" s="2">
         <v>6242.8</v>
       </c>
-      <c r="K19" s="5">
+      <c r="K19" s="2">
         <f>((K4+K3) - J19)</f>
         <v>9.3999999999996362</v>
       </c>
-      <c r="L19" s="9">
+      <c r="L19" s="6">
         <f t="shared" si="2"/>
         <v>3.7599999999998546</v>
       </c>
-      <c r="M19" s="5">
+      <c r="M19" s="2">
         <v>6164.8</v>
       </c>
-      <c r="N19" s="5">
+      <c r="N19" s="2">
         <f>((K4+K3) - M19)</f>
         <v>87.399999999999636</v>
       </c>
-      <c r="O19" s="9">
+      <c r="O19" s="6">
         <f t="shared" si="3"/>
         <v>34.959999999999852</v>
       </c>
       <c r="Q19">
         <v>60</v>
       </c>
-      <c r="R19" s="5">
+      <c r="R19" s="2">
         <v>6728.4</v>
       </c>
-      <c r="S19" s="5">
+      <c r="S19" s="2">
         <f>((S4+S3) - R19)</f>
         <v>23.300000000000182</v>
       </c>
-      <c r="T19" s="9">
+      <c r="T19" s="6">
         <f t="shared" si="4"/>
         <v>3.1066666666666909</v>
       </c>
-      <c r="U19" s="5">
+      <c r="U19" s="2">
         <v>6610.2</v>
       </c>
-      <c r="V19" s="5">
+      <c r="V19" s="2">
         <f>((S4+S3) - U19)</f>
         <v>141.5</v>
       </c>
-      <c r="W19" s="9">
+      <c r="W19" s="6">
         <f t="shared" si="5"/>
         <v>18.866666666666667</v>
       </c>
@@ -7343,75 +7987,75 @@
       <c r="A20">
         <v>65</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="2">
         <v>6071.8</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="2">
         <f>((C4+C3) - B20)</f>
         <v>3.0999999999994543</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="6">
         <f t="shared" si="0"/>
         <v>4.1333333333326054</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="2">
         <v>6018.8</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F20" s="2">
         <f>((C4+C3) - E20)</f>
         <v>56.099999999999454</v>
       </c>
-      <c r="G20" s="9">
+      <c r="G20" s="6">
         <f t="shared" si="1"/>
         <v>74.799999999999272</v>
       </c>
       <c r="I20">
         <v>65</v>
       </c>
-      <c r="J20" s="5">
+      <c r="J20" s="2">
         <v>6242</v>
       </c>
-      <c r="K20" s="5">
+      <c r="K20" s="2">
         <f>((K4+K3) - J20)</f>
         <v>10.199999999999818</v>
       </c>
-      <c r="L20" s="9">
+      <c r="L20" s="6">
         <f t="shared" si="2"/>
         <v>4.0799999999999272</v>
       </c>
-      <c r="M20" s="5">
+      <c r="M20" s="2">
         <v>6159.7</v>
       </c>
-      <c r="N20" s="5">
+      <c r="N20" s="2">
         <f>((K4+K3) - M20)</f>
         <v>92.5</v>
       </c>
-      <c r="O20" s="9">
+      <c r="O20" s="6">
         <f t="shared" si="3"/>
         <v>37</v>
       </c>
       <c r="Q20">
         <v>65</v>
       </c>
-      <c r="R20" s="5">
+      <c r="R20" s="2">
         <v>6726.9</v>
       </c>
-      <c r="S20" s="5">
+      <c r="S20" s="2">
         <f>((S4+S3) - R20)</f>
         <v>24.800000000000182</v>
       </c>
-      <c r="T20" s="9">
+      <c r="T20" s="6">
         <f t="shared" si="4"/>
         <v>3.3066666666666911</v>
       </c>
-      <c r="U20" s="5">
+      <c r="U20" s="2">
         <v>6602.5</v>
       </c>
-      <c r="V20" s="5">
+      <c r="V20" s="2">
         <f>((S4+S3) - U20)</f>
         <v>149.19999999999982</v>
       </c>
-      <c r="W20" s="9">
+      <c r="W20" s="6">
         <f t="shared" si="5"/>
         <v>19.89333333333331</v>
       </c>
@@ -7420,75 +8064,75 @@
       <c r="A21">
         <v>70</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="2">
         <v>6071.4</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="2">
         <f>((C4+C3) - B21)</f>
         <v>3.5</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D21" s="6">
         <f t="shared" si="0"/>
         <v>4.666666666666667</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="2">
         <v>6015.4</v>
       </c>
-      <c r="F21" s="5">
+      <c r="F21" s="2">
         <f>((C4+C3) - E21)</f>
         <v>59.5</v>
       </c>
-      <c r="G21" s="9">
+      <c r="G21" s="6">
         <f t="shared" si="1"/>
         <v>79.333333333333329</v>
       </c>
       <c r="I21">
         <v>70</v>
       </c>
-      <c r="J21" s="5">
+      <c r="J21" s="2">
         <v>6241.2</v>
       </c>
-      <c r="K21" s="5">
+      <c r="K21" s="2">
         <f>((K4+K3) - J21)</f>
         <v>11</v>
       </c>
-      <c r="L21" s="9">
+      <c r="L21" s="6">
         <f t="shared" si="2"/>
         <v>4.3999999999999995</v>
       </c>
-      <c r="M21" s="5">
+      <c r="M21" s="2">
         <v>6155.2</v>
       </c>
-      <c r="N21" s="5">
+      <c r="N21" s="2">
         <f>((K4+K3) - M21)</f>
         <v>97</v>
       </c>
-      <c r="O21" s="9">
+      <c r="O21" s="6">
         <f t="shared" si="3"/>
         <v>38.800000000000004</v>
       </c>
       <c r="Q21">
         <v>70</v>
       </c>
-      <c r="R21" s="5">
+      <c r="R21" s="2">
         <v>6725.6</v>
       </c>
-      <c r="S21" s="5">
+      <c r="S21" s="2">
         <f>((S4+S3) - R21)</f>
         <v>26.099999999999454</v>
       </c>
-      <c r="T21" s="9">
+      <c r="T21" s="6">
         <f t="shared" si="4"/>
         <v>3.4799999999999267</v>
       </c>
-      <c r="U21" s="5">
+      <c r="U21" s="2">
         <v>6593.5</v>
       </c>
-      <c r="V21" s="5">
+      <c r="V21" s="2">
         <f>((S4+S3) - U21)</f>
         <v>158.19999999999982</v>
       </c>
-      <c r="W21" s="9">
+      <c r="W21" s="6">
         <f t="shared" si="5"/>
         <v>21.093333333333309</v>
       </c>
@@ -7497,75 +8141,75 @@
       <c r="A22">
         <v>75</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="2">
         <v>6070.9</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="2">
         <f>((C4+C3) - B22)</f>
         <v>4</v>
       </c>
-      <c r="D22" s="9">
+      <c r="D22" s="6">
         <f t="shared" si="0"/>
         <v>5.3333333333333339</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="2">
         <v>6012.2</v>
       </c>
-      <c r="F22" s="5">
+      <c r="F22" s="2">
         <f>((C4+C3) - E22)</f>
         <v>62.699999999999818</v>
       </c>
-      <c r="G22" s="9">
+      <c r="G22" s="6">
         <f t="shared" si="1"/>
         <v>83.599999999999753</v>
       </c>
       <c r="I22">
         <v>75</v>
       </c>
-      <c r="J22" s="5">
+      <c r="J22" s="2">
         <v>6240.4</v>
       </c>
-      <c r="K22" s="5">
+      <c r="K22" s="2">
         <f>((K4+K3) - J22)</f>
         <v>11.800000000000182</v>
       </c>
-      <c r="L22" s="9">
+      <c r="L22" s="6">
         <f t="shared" si="2"/>
         <v>4.7200000000000726</v>
       </c>
-      <c r="M22" s="5">
+      <c r="M22" s="2">
         <v>6150.5</v>
       </c>
-      <c r="N22" s="5">
+      <c r="N22" s="2">
         <f>((K4+K3) - M22)</f>
         <v>101.69999999999982</v>
       </c>
-      <c r="O22" s="9">
+      <c r="O22" s="6">
         <f t="shared" si="3"/>
         <v>40.679999999999929</v>
       </c>
       <c r="Q22">
         <v>75</v>
       </c>
-      <c r="R22" s="5">
+      <c r="R22" s="2">
         <v>6724.2</v>
       </c>
-      <c r="S22" s="5">
+      <c r="S22" s="2">
         <f>((S4+S3) - R22)</f>
         <v>27.5</v>
       </c>
-      <c r="T22" s="9">
+      <c r="T22" s="6">
         <f t="shared" si="4"/>
         <v>3.6666666666666665</v>
       </c>
-      <c r="U22" s="5">
+      <c r="U22" s="2">
         <v>6587.9</v>
       </c>
-      <c r="V22" s="5">
+      <c r="V22" s="2">
         <f>((S4+S3) - U22)</f>
         <v>163.80000000000018</v>
       </c>
-      <c r="W22" s="9">
+      <c r="W22" s="6">
         <f t="shared" si="5"/>
         <v>21.840000000000025</v>
       </c>
@@ -7574,75 +8218,75 @@
       <c r="A23">
         <v>80</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="2">
         <v>6070.3</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="2">
         <f>((C4+C3) - B23)</f>
         <v>4.5999999999994543</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23" s="6">
         <f t="shared" si="0"/>
         <v>6.1333333333326054</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="2">
         <v>6009.7</v>
       </c>
-      <c r="F23" s="5">
+      <c r="F23" s="2">
         <f>((C4+C3) - E23)</f>
         <v>65.199999999999818</v>
       </c>
-      <c r="G23" s="9">
+      <c r="G23" s="6">
         <f t="shared" si="1"/>
         <v>86.933333333333096</v>
       </c>
       <c r="I23">
         <v>80</v>
       </c>
-      <c r="J23" s="5">
+      <c r="J23" s="2">
         <v>6239.5</v>
       </c>
-      <c r="K23" s="5">
+      <c r="K23" s="2">
         <f>((K4+K3) - J23)</f>
         <v>12.699999999999818</v>
       </c>
-      <c r="L23" s="9">
+      <c r="L23" s="6">
         <f t="shared" si="2"/>
         <v>5.0799999999999272</v>
       </c>
-      <c r="M23" s="5">
+      <c r="M23" s="2">
         <v>6146</v>
       </c>
-      <c r="N23" s="5">
+      <c r="N23" s="2">
         <f>((K4+K3) - M23)</f>
         <v>106.19999999999982</v>
       </c>
-      <c r="O23" s="9">
+      <c r="O23" s="6">
         <f t="shared" si="3"/>
         <v>42.479999999999926</v>
       </c>
       <c r="Q23">
         <v>80</v>
       </c>
-      <c r="R23" s="5">
+      <c r="R23" s="2">
         <v>6723.1</v>
       </c>
-      <c r="S23" s="5">
+      <c r="S23" s="2">
         <f>((S4+S3) - R23)</f>
         <v>28.599999999999454</v>
       </c>
-      <c r="T23" s="9">
+      <c r="T23" s="6">
         <f t="shared" si="4"/>
         <v>3.8133333333332602</v>
       </c>
-      <c r="U23" s="5">
+      <c r="U23" s="2">
         <v>6581</v>
       </c>
-      <c r="V23" s="5">
+      <c r="V23" s="2">
         <f>((S4+S3) - U23)</f>
         <v>170.69999999999982</v>
       </c>
-      <c r="W23" s="9">
+      <c r="W23" s="6">
         <f t="shared" si="5"/>
         <v>22.759999999999973</v>
       </c>
@@ -7651,75 +8295,75 @@
       <c r="A24">
         <v>85</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="2">
         <v>6069.9</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="2">
         <f>((C4+C3) - B24)</f>
         <v>5</v>
       </c>
-      <c r="D24" s="9">
+      <c r="D24" s="6">
         <f t="shared" si="0"/>
         <v>6.666666666666667</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="2">
         <v>6007.1</v>
       </c>
-      <c r="F24" s="5">
+      <c r="F24" s="2">
         <f>((C4+C3) - E24)</f>
         <v>67.799999999999272</v>
       </c>
-      <c r="G24" s="9">
+      <c r="G24" s="6">
         <f t="shared" si="1"/>
         <v>90.399999999999025</v>
       </c>
       <c r="I24">
         <v>85</v>
       </c>
-      <c r="J24" s="5">
+      <c r="J24" s="2">
         <v>6238.8</v>
       </c>
-      <c r="K24" s="5">
+      <c r="K24" s="2">
         <f>((K4+K3) - J24)</f>
         <v>13.399999999999636</v>
       </c>
-      <c r="L24" s="9">
+      <c r="L24" s="6">
         <f t="shared" si="2"/>
         <v>5.3599999999998547</v>
       </c>
-      <c r="M24" s="5">
+      <c r="M24" s="2">
         <v>6141.7</v>
       </c>
-      <c r="N24" s="5">
+      <c r="N24" s="2">
         <f>((K4+K3) - M24)</f>
         <v>110.5</v>
       </c>
-      <c r="O24" s="9">
+      <c r="O24" s="6">
         <f t="shared" si="3"/>
         <v>44.2</v>
       </c>
       <c r="Q24">
         <v>85</v>
       </c>
-      <c r="R24" s="5">
+      <c r="R24" s="2">
         <v>6722.1</v>
       </c>
-      <c r="S24" s="5">
+      <c r="S24" s="2">
         <f>((S4+S3) - R24)</f>
         <v>29.599999999999454</v>
       </c>
-      <c r="T24" s="9">
+      <c r="T24" s="6">
         <f t="shared" si="4"/>
         <v>3.9466666666665944</v>
       </c>
-      <c r="U24" s="5">
+      <c r="U24" s="2">
         <v>6574.2</v>
       </c>
-      <c r="V24" s="5">
+      <c r="V24" s="2">
         <f>((S4+S3) - U24)</f>
         <v>177.5</v>
       </c>
-      <c r="W24" s="9">
+      <c r="W24" s="6">
         <f t="shared" si="5"/>
         <v>23.666666666666668</v>
       </c>
@@ -7728,75 +8372,75 @@
       <c r="A25">
         <v>90</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="2">
         <v>6069.3</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="2">
         <f>((C4+C3) - B25)</f>
         <v>5.5999999999994543</v>
       </c>
-      <c r="D25" s="9">
+      <c r="D25" s="6">
         <f t="shared" si="0"/>
         <v>7.4666666666659385</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E25" s="2">
         <v>6006.8</v>
       </c>
-      <c r="F25" s="5">
+      <c r="F25" s="2">
         <f>((C4+C3) - E25)</f>
         <v>68.099999999999454</v>
       </c>
-      <c r="G25" s="9">
+      <c r="G25" s="6">
         <f t="shared" si="1"/>
         <v>90.799999999999272</v>
       </c>
       <c r="I25">
         <v>90</v>
       </c>
-      <c r="J25" s="5">
+      <c r="J25" s="2">
         <v>6237.8</v>
       </c>
-      <c r="K25" s="5">
+      <c r="K25" s="2">
         <f>((K4+K3) - J25)</f>
         <v>14.399999999999636</v>
       </c>
-      <c r="L25" s="9">
+      <c r="L25" s="6">
         <f t="shared" si="2"/>
         <v>5.759999999999855</v>
       </c>
-      <c r="M25" s="5">
+      <c r="M25" s="2">
         <v>6137.3</v>
       </c>
-      <c r="N25" s="5">
+      <c r="N25" s="2">
         <f>((K4+K3) - M25)</f>
         <v>114.89999999999964</v>
       </c>
-      <c r="O25" s="9">
+      <c r="O25" s="6">
         <f t="shared" si="3"/>
         <v>45.959999999999859</v>
       </c>
       <c r="Q25">
         <v>90</v>
       </c>
-      <c r="R25" s="5">
+      <c r="R25" s="2">
         <v>6721</v>
       </c>
-      <c r="S25" s="5">
+      <c r="S25" s="2">
         <f>((S4+S3) - R25)</f>
         <v>30.699999999999818</v>
       </c>
-      <c r="T25" s="9">
+      <c r="T25" s="6">
         <f t="shared" si="4"/>
         <v>4.0933333333333088</v>
       </c>
-      <c r="U25" s="5">
+      <c r="U25" s="2">
         <v>6567.3</v>
       </c>
-      <c r="V25" s="5">
+      <c r="V25" s="2">
         <f>((S4+S3) - U25)</f>
         <v>184.39999999999964</v>
       </c>
-      <c r="W25" s="9">
+      <c r="W25" s="6">
         <f t="shared" si="5"/>
         <v>24.586666666666616</v>
       </c>
@@ -7805,75 +8449,75 @@
       <c r="A26">
         <v>95</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="2">
         <v>6068.8</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="2">
         <f>((C4+C3) - B26)</f>
         <v>6.0999999999994543</v>
       </c>
-      <c r="D26" s="9">
+      <c r="D26" s="6">
         <f t="shared" si="0"/>
         <v>8.1333333333326063</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E26" s="2">
         <v>6006.8</v>
       </c>
-      <c r="F26" s="5">
+      <c r="F26" s="2">
         <f>((C4+C3) - E26)</f>
         <v>68.099999999999454</v>
       </c>
-      <c r="G26" s="9">
+      <c r="G26" s="6">
         <f t="shared" si="1"/>
         <v>90.799999999999272</v>
       </c>
       <c r="I26">
         <v>95</v>
       </c>
-      <c r="J26" s="5">
+      <c r="J26" s="2">
         <v>6237.2</v>
       </c>
-      <c r="K26" s="5">
+      <c r="K26" s="2">
         <f>((K4+K3) - J26)</f>
         <v>15</v>
       </c>
-      <c r="L26" s="9">
+      <c r="L26" s="6">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="M26" s="5">
+      <c r="M26" s="2">
         <v>6133.2</v>
       </c>
-      <c r="N26" s="5">
+      <c r="N26" s="2">
         <f>((K4+K3) - M26)</f>
         <v>119</v>
       </c>
-      <c r="O26" s="9">
+      <c r="O26" s="6">
         <f t="shared" si="3"/>
         <v>47.599999999999994</v>
       </c>
       <c r="Q26">
         <v>95</v>
       </c>
-      <c r="R26" s="5">
+      <c r="R26" s="2">
         <v>6719.6</v>
       </c>
-      <c r="S26" s="5">
+      <c r="S26" s="2">
         <f>((S4+S3) - R26)</f>
         <v>32.099999999999454</v>
       </c>
-      <c r="T26" s="9">
+      <c r="T26" s="6">
         <f t="shared" si="4"/>
         <v>4.2799999999999265</v>
       </c>
-      <c r="U26" s="5">
+      <c r="U26" s="2">
         <v>6560.7</v>
       </c>
-      <c r="V26" s="5">
+      <c r="V26" s="2">
         <f>((S4+S3) - U26)</f>
         <v>191</v>
       </c>
-      <c r="W26" s="9">
+      <c r="W26" s="6">
         <f t="shared" si="5"/>
         <v>25.466666666666665</v>
       </c>
@@ -7882,75 +8526,75 @@
       <c r="A27">
         <v>100</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B27" s="2">
         <v>6068.2</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C27" s="2">
         <f>((C4+C3) - B27)</f>
         <v>6.6999999999998181</v>
       </c>
-      <c r="D27" s="9">
+      <c r="D27" s="6">
         <f t="shared" si="0"/>
         <v>8.9333333333330902</v>
       </c>
-      <c r="E27" s="5">
+      <c r="E27" s="2">
         <v>6006.8</v>
       </c>
-      <c r="F27" s="5">
+      <c r="F27" s="2">
         <f>((C4+C3) - E27)</f>
         <v>68.099999999999454</v>
       </c>
-      <c r="G27" s="9">
+      <c r="G27" s="6">
         <f t="shared" si="1"/>
         <v>90.799999999999272</v>
       </c>
       <c r="I27">
         <v>100</v>
       </c>
-      <c r="J27" s="5">
+      <c r="J27" s="2">
         <v>6236.4</v>
       </c>
-      <c r="K27" s="5">
+      <c r="K27" s="2">
         <f>((K4+K3) - J27)</f>
         <v>15.800000000000182</v>
       </c>
-      <c r="L27" s="9">
+      <c r="L27" s="6">
         <f t="shared" si="2"/>
         <v>6.3200000000000731</v>
       </c>
-      <c r="M27" s="5">
+      <c r="M27" s="2">
         <v>6129</v>
       </c>
-      <c r="N27" s="5">
+      <c r="N27" s="2">
         <f>((K4+K3) - M27)</f>
         <v>123.19999999999982</v>
       </c>
-      <c r="O27" s="9">
+      <c r="O27" s="6">
         <f t="shared" si="3"/>
         <v>49.27999999999993</v>
       </c>
       <c r="Q27">
         <v>100</v>
       </c>
-      <c r="R27" s="5">
+      <c r="R27" s="2">
         <v>6718.3</v>
       </c>
-      <c r="S27" s="5">
+      <c r="S27" s="2">
         <f>((S4+S3) - R27)</f>
         <v>33.399999999999636</v>
       </c>
-      <c r="T27" s="9">
+      <c r="T27" s="6">
         <f t="shared" si="4"/>
         <v>4.4533333333332852</v>
       </c>
-      <c r="U27" s="5">
+      <c r="U27" s="2">
         <v>6554.2</v>
       </c>
-      <c r="V27" s="5">
+      <c r="V27" s="2">
         <f>((S4+S3) - U27)</f>
         <v>197.5</v>
       </c>
-      <c r="W27" s="9">
+      <c r="W27" s="6">
         <f t="shared" si="5"/>
         <v>26.333333333333332</v>
       </c>

</xml_diff>